<commit_message>
Pass SkillConfig as UpgradeOption from SkillManager to UpgradeMenuManager
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/skill.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/skill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698AB46B-40FB-417E-9014-D67613D35E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F945C02F-D4EC-43AF-A05E-A7EEF48B3B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>level 1 des</t>
-  </si>
-  <si>
     <t>level 2 des</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>ATTACK_DECREASE</t>
+  </si>
+  <si>
+    <t>level 4 des</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1"/>
@@ -368,6 +368,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -648,7 +649,7 @@
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -681,7 +682,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="17"/>
       <c r="H1" s="12" t="s">
@@ -717,7 +718,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>16</v>
@@ -726,7 +727,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>16</v>
@@ -757,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -766,10 +767,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="13" t="s">
@@ -836,7 +837,7 @@
     </row>
     <row r="5" spans="1:28">
       <c r="B5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
@@ -845,65 +846,65 @@
         <v>12</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="14">
         <v>8</v>
       </c>
       <c r="H5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:28">
       <c r="F6" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="10">
         <v>3</v>
       </c>
       <c r="H6" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6">
         <v>10</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="21" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:28">
       <c r="F7" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="11">
         <v>0.15</v>
       </c>
       <c r="H7" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J7">
         <v>4</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>19</v>
+      <c r="K7" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:28">

</xml_diff>

<commit_message>
Fix the exception when upgrading a passive skill
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/skill.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/skill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tigersun/Code/GobangAdventure/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2668D73-1FBA-B741-992B-38AD37875327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA12CA-3619-9546-8A78-746C14E71054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1092,7 +1092,7 @@
         <v>59</v>
       </c>
       <c r="G10" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="13">
         <v>1</v>
@@ -1206,7 +1206,7 @@
         <v>59</v>
       </c>
       <c r="G16" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="13">
         <v>1</v>
@@ -1320,7 +1320,7 @@
         <v>59</v>
       </c>
       <c r="G22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="13">
         <v>1</v>
@@ -1434,7 +1434,7 @@
         <v>59</v>
       </c>
       <c r="G28" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="13">
         <v>1</v>
@@ -1547,7 +1547,7 @@
         <v>59</v>
       </c>
       <c r="G34" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="21">
         <v>1</v>

</xml_diff>